<commit_message>
Added ability to edit existing entries on excel sheet
</commit_message>
<xml_diff>
--- a/food_list.xlsx
+++ b/food_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:H166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Restaurant</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 2</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -459,676 +474,1081 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve">McDonald's </t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Freddy's</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Taco Bell</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>Pizza Hut</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Domino's</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Prado's</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>Mission Taco</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Street Beanz</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="F9" t="n">
         <v>4</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>Sbux</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="F10" t="n">
         <v>4</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Alpha and Omega</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="F11" t="n">
         <v>4</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>Crooked Tree</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="F12" t="n">
         <v>4</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t xml:space="preserve">Piccaso's </t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="F13" t="n">
         <v>4</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>Jimmy John's</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>Kaldi</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="F15" t="n">
         <v>4</v>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Chick-fil-a</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>Cane's</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>Crazy Bowls and Wraps</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>Sauce on the Side</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t xml:space="preserve">Dewey's </t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>2</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>Sugarfire</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>2</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>Texas Roadhouse</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>2</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>Salt and Smoke</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>22</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>Cold Stone</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="F24" t="n">
         <v>3</v>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" t="n">
+        <v>23</v>
+      </c>
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>Culver's</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" t="n">
+        <v>24</v>
+      </c>
+      <c r="C26" t="n">
+        <v>24</v>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>Culver's</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="F26" t="n">
         <v>3</v>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" t="n">
+        <v>25</v>
+      </c>
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>25</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>Freddy's</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="F27" t="n">
         <v>3</v>
       </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="n">
+        <v>26</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t xml:space="preserve">McDonald's </t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="F28" t="n">
         <v>3</v>
       </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" t="n">
+        <v>27</v>
+      </c>
+      <c r="C29" t="n">
+        <v>27</v>
+      </c>
+      <c r="D29" t="n">
+        <v>27</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t xml:space="preserve">Clementine's </t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="F29" t="n">
         <v>3</v>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" t="n">
+        <v>28</v>
+      </c>
+      <c r="C30" t="n">
+        <v>28</v>
+      </c>
+      <c r="D30" t="n">
+        <v>28</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>Fritz's</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="F30" t="n">
         <v>3</v>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" t="n">
+        <v>29</v>
+      </c>
+      <c r="C31" t="n">
+        <v>29</v>
+      </c>
+      <c r="D31" t="n">
+        <v>29</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>Fitz's</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="F31" t="n">
         <v>3</v>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>30</v>
+      </c>
+      <c r="D32" t="n">
+        <v>30</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>Panera</t>
         </is>
       </c>
-      <c r="C32" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" t="n">
+        <v>31</v>
+      </c>
+      <c r="C33" t="n">
+        <v>31</v>
+      </c>
+      <c r="D33" t="n">
+        <v>31</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>Steak 'n Shake</t>
         </is>
       </c>
-      <c r="C33" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" t="n">
+        <v>32</v>
+      </c>
+      <c r="C34" t="n">
+        <v>32</v>
+      </c>
+      <c r="D34" t="n">
+        <v>32</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>Chimi's</t>
         </is>
       </c>
-      <c r="C34" t="n">
-        <v>2</v>
-      </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" t="n">
+        <v>33</v>
+      </c>
+      <c r="C35" t="n">
+        <v>33</v>
+      </c>
+      <c r="D35" t="n">
+        <v>33</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>McAllister's</t>
         </is>
       </c>
-      <c r="C35" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" t="n">
+        <v>34</v>
+      </c>
+      <c r="C36" t="n">
+        <v>34</v>
+      </c>
+      <c r="D36" t="n">
+        <v>34</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>Red Robin</t>
         </is>
       </c>
-      <c r="C36" t="n">
-        <v>2</v>
-      </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" t="n">
+        <v>35</v>
+      </c>
+      <c r="C37" t="n">
+        <v>35</v>
+      </c>
+      <c r="D37" t="n">
+        <v>35</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>Five Guys</t>
         </is>
       </c>
-      <c r="C37" t="n">
-        <v>2</v>
-      </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" t="n">
+        <v>36</v>
+      </c>
+      <c r="C38" t="n">
+        <v>36</v>
+      </c>
+      <c r="D38" t="n">
+        <v>36</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>Hi-Pointe Drive In</t>
         </is>
       </c>
-      <c r="C38" t="n">
-        <v>2</v>
-      </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" t="n">
+        <v>37</v>
+      </c>
+      <c r="C39" t="n">
+        <v>37</v>
+      </c>
+      <c r="D39" t="n">
+        <v>37</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>Waffle House</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="F39" t="n">
         <v>6</v>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" t="n">
+        <v>38</v>
+      </c>
+      <c r="C40" t="n">
+        <v>38</v>
+      </c>
+      <c r="D40" t="n">
+        <v>38</v>
+      </c>
+      <c r="E40" t="inlineStr">
         <is>
           <t xml:space="preserve">Denny's </t>
         </is>
       </c>
-      <c r="C40" t="n">
+      <c r="F40" t="n">
         <v>6</v>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" t="n">
+        <v>39</v>
+      </c>
+      <c r="C41" t="n">
+        <v>39</v>
+      </c>
+      <c r="D41" t="n">
+        <v>39</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>IHop</t>
         </is>
       </c>
-      <c r="C41" t="n">
+      <c r="F41" t="n">
         <v>6</v>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" t="n">
+        <v>40</v>
+      </c>
+      <c r="C42" t="n">
+        <v>40</v>
+      </c>
+      <c r="D42" t="n">
+        <v>40</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t xml:space="preserve">Bob Evan's </t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="F42" t="n">
         <v>6</v>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" t="n">
+        <v>41</v>
+      </c>
+      <c r="C43" t="n">
+        <v>41</v>
+      </c>
+      <c r="D43" t="n">
+        <v>41</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>Panda Express</t>
         </is>
       </c>
-      <c r="C43" t="n">
-        <v>1</v>
-      </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" t="n">
+        <v>42</v>
+      </c>
+      <c r="C44" t="n">
+        <v>42</v>
+      </c>
+      <c r="D44" t="n">
+        <v>42</v>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>Burger King</t>
         </is>
       </c>
-      <c r="C44" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" t="n">
+        <v>43</v>
+      </c>
+      <c r="C45" t="n">
+        <v>43</v>
+      </c>
+      <c r="D45" t="n">
+        <v>43</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>Soulard Gyro</t>
         </is>
       </c>
-      <c r="C45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" t="n">
+        <v>44</v>
+      </c>
+      <c r="C46" t="n">
+        <v>44</v>
+      </c>
+      <c r="D46" t="n">
+        <v>44</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>Sonic</t>
         </is>
       </c>
-      <c r="C46" t="n">
-        <v>1</v>
-      </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
         <is>
           <t>Fast food=1</t>
         </is>
@@ -1138,16 +1558,25 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" t="n">
+        <v>45</v>
+      </c>
+      <c r="C47" t="n">
+        <v>45</v>
+      </c>
+      <c r="D47" t="n">
+        <v>45</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>Popeyes</t>
         </is>
       </c>
-      <c r="C47" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
         <is>
           <t>Dine in=2</t>
         </is>
@@ -1157,16 +1586,25 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" t="n">
+        <v>46</v>
+      </c>
+      <c r="C48" t="n">
+        <v>46</v>
+      </c>
+      <c r="D48" t="n">
+        <v>46</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>Qdoba</t>
         </is>
       </c>
-      <c r="C48" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
         <is>
           <t xml:space="preserve">Dessert=3 </t>
         </is>
@@ -1176,16 +1614,25 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" t="n">
+        <v>47</v>
+      </c>
+      <c r="C49" t="n">
+        <v>47</v>
+      </c>
+      <c r="D49" t="n">
+        <v>47</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>Chipotle</t>
         </is>
       </c>
-      <c r="C49" t="n">
-        <v>1</v>
-      </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
         <is>
           <t>Coffee=4</t>
         </is>
@@ -1195,16 +1642,25 @@
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" t="n">
+        <v>48</v>
+      </c>
+      <c r="C50" t="n">
+        <v>48</v>
+      </c>
+      <c r="D50" t="n">
+        <v>48</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>Dairy Queen</t>
         </is>
       </c>
-      <c r="C50" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
         <is>
           <t>Alcohol=5</t>
         </is>
@@ -1214,1696 +1670,2773 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" t="n">
+        <v>49</v>
+      </c>
+      <c r="C51" t="n">
+        <v>49</v>
+      </c>
+      <c r="D51" t="n">
+        <v>49</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>Marco's Pizza</t>
         </is>
       </c>
-      <c r="C51" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B52" t="n">
+        <v>50</v>
+      </c>
+      <c r="C52" t="n">
+        <v>50</v>
+      </c>
+      <c r="D52" t="n">
+        <v>50</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>Lion's Choice</t>
         </is>
       </c>
-      <c r="C52" t="n">
-        <v>1</v>
-      </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B53" t="n">
+        <v>51</v>
+      </c>
+      <c r="C53" t="n">
+        <v>51</v>
+      </c>
+      <c r="D53" t="n">
+        <v>51</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>Sushi Ai</t>
         </is>
       </c>
-      <c r="C53" t="n">
-        <v>2</v>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" t="n">
+        <v>52</v>
+      </c>
+      <c r="C54" t="n">
+        <v>52</v>
+      </c>
+      <c r="D54" t="n">
+        <v>52</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>54th Street</t>
         </is>
       </c>
-      <c r="C54" t="n">
-        <v>2</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="n">
+        <v>2</v>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" t="n">
+        <v>53</v>
+      </c>
+      <c r="C55" t="n">
+        <v>53</v>
+      </c>
+      <c r="D55" t="n">
+        <v>53</v>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>The Tattooed Dog</t>
         </is>
       </c>
-      <c r="C55" t="n">
-        <v>2</v>
-      </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="n">
+        <v>2</v>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B56" t="n">
+        <v>54</v>
+      </c>
+      <c r="C56" t="n">
+        <v>54</v>
+      </c>
+      <c r="D56" t="n">
+        <v>54</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>Applebee's</t>
         </is>
       </c>
-      <c r="C56" t="n">
-        <v>2</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="n">
+        <v>2</v>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B57" t="n">
+        <v>55</v>
+      </c>
+      <c r="C57" t="n">
+        <v>55</v>
+      </c>
+      <c r="D57" t="n">
+        <v>55</v>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>Chili's</t>
         </is>
       </c>
-      <c r="C57" t="n">
-        <v>2</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="n">
+        <v>2</v>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B58" t="n">
+        <v>56</v>
+      </c>
+      <c r="C58" t="n">
+        <v>56</v>
+      </c>
+      <c r="D58" t="n">
+        <v>56</v>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>Mod Pizza</t>
         </is>
       </c>
-      <c r="C58" t="n">
-        <v>1</v>
-      </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B59" t="n">
+        <v>57</v>
+      </c>
+      <c r="C59" t="n">
+        <v>57</v>
+      </c>
+      <c r="D59" t="n">
+        <v>57</v>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t>Krumbly Burger</t>
         </is>
       </c>
-      <c r="C59" t="n">
-        <v>1</v>
-      </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B60" t="n">
+        <v>58</v>
+      </c>
+      <c r="C60" t="n">
+        <v>58</v>
+      </c>
+      <c r="D60" t="n">
+        <v>58</v>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>Slim Chickens</t>
         </is>
       </c>
-      <c r="C60" t="n">
-        <v>1</v>
-      </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B61" t="n">
+        <v>59</v>
+      </c>
+      <c r="C61" t="n">
+        <v>59</v>
+      </c>
+      <c r="D61" t="n">
+        <v>59</v>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>Thai Kitchen</t>
         </is>
       </c>
-      <c r="C61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B62" t="n">
+        <v>60</v>
+      </c>
+      <c r="C62" t="n">
+        <v>60</v>
+      </c>
+      <c r="D62" t="n">
+        <v>60</v>
+      </c>
+      <c r="E62" t="inlineStr">
         <is>
           <t>Balkan Treat Box</t>
         </is>
       </c>
-      <c r="C62" t="n">
-        <v>2</v>
-      </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="n">
+        <v>2</v>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B63" t="n">
+        <v>61</v>
+      </c>
+      <c r="C63" t="n">
+        <v>61</v>
+      </c>
+      <c r="D63" t="n">
+        <v>61</v>
+      </c>
+      <c r="E63" t="inlineStr">
         <is>
           <t>Olive Garden</t>
         </is>
       </c>
-      <c r="C63" t="n">
-        <v>2</v>
-      </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>2</v>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B64" t="n">
+        <v>62</v>
+      </c>
+      <c r="C64" t="n">
+        <v>62</v>
+      </c>
+      <c r="D64" t="n">
+        <v>62</v>
+      </c>
+      <c r="E64" t="inlineStr">
         <is>
           <t xml:space="preserve">El Tio Pepe </t>
         </is>
       </c>
-      <c r="C64" t="n">
-        <v>2</v>
-      </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B65" t="n">
+        <v>63</v>
+      </c>
+      <c r="C65" t="n">
+        <v>63</v>
+      </c>
+      <c r="D65" t="n">
+        <v>63</v>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t xml:space="preserve">Stefanina's </t>
         </is>
       </c>
-      <c r="C65" t="n">
-        <v>1</v>
-      </c>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B66" t="n">
+        <v>64</v>
+      </c>
+      <c r="C66" t="n">
+        <v>64</v>
+      </c>
+      <c r="D66" t="n">
+        <v>64</v>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>Walnut Grill</t>
         </is>
       </c>
-      <c r="C66" t="n">
-        <v>2</v>
-      </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="n">
+        <v>2</v>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B67" t="n">
+        <v>65</v>
+      </c>
+      <c r="C67" t="n">
+        <v>65</v>
+      </c>
+      <c r="D67" t="n">
+        <v>65</v>
+      </c>
+      <c r="E67" t="inlineStr">
         <is>
           <t>Dunkin</t>
         </is>
       </c>
-      <c r="C67" t="n">
+      <c r="F67" t="n">
         <v>4</v>
       </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B68" t="n">
+        <v>66</v>
+      </c>
+      <c r="C68" t="n">
+        <v>66</v>
+      </c>
+      <c r="D68" t="n">
+        <v>66</v>
+      </c>
+      <c r="E68" t="inlineStr">
         <is>
           <t>Krispy Kreme</t>
         </is>
       </c>
-      <c r="C68" t="n">
+      <c r="F68" t="n">
         <v>6</v>
       </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B69" t="n">
+        <v>67</v>
+      </c>
+      <c r="C69" t="n">
+        <v>67</v>
+      </c>
+      <c r="D69" t="n">
+        <v>67</v>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>Old Town Donuts</t>
         </is>
       </c>
-      <c r="C69" t="n">
+      <c r="F69" t="n">
         <v>6</v>
       </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B70" t="n">
+        <v>68</v>
+      </c>
+      <c r="C70" t="n">
+        <v>68</v>
+      </c>
+      <c r="D70" t="n">
+        <v>68</v>
+      </c>
+      <c r="E70" t="inlineStr">
         <is>
           <t>Goodcent's</t>
         </is>
       </c>
-      <c r="C70" t="n">
-        <v>1</v>
-      </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B71" t="n">
+        <v>69</v>
+      </c>
+      <c r="C71" t="n">
+        <v>69</v>
+      </c>
+      <c r="D71" t="n">
+        <v>69</v>
+      </c>
+      <c r="E71" t="inlineStr">
         <is>
           <t>Heaven Scent</t>
         </is>
       </c>
-      <c r="C71" t="n">
+      <c r="F71" t="n">
         <v>6</v>
       </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B72" t="n">
+        <v>70</v>
+      </c>
+      <c r="C72" t="n">
+        <v>70</v>
+      </c>
+      <c r="D72" t="n">
+        <v>70</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>Einstein's</t>
         </is>
       </c>
-      <c r="C72" t="n">
+      <c r="F72" t="n">
         <v>6</v>
       </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B73" t="n">
+        <v>71</v>
+      </c>
+      <c r="C73" t="n">
+        <v>71</v>
+      </c>
+      <c r="D73" t="n">
+        <v>71</v>
+      </c>
+      <c r="E73" t="inlineStr">
         <is>
           <t>Andy's</t>
         </is>
       </c>
-      <c r="C73" t="n">
+      <c r="F73" t="n">
         <v>3</v>
       </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B74" t="n">
+        <v>72</v>
+      </c>
+      <c r="C74" t="n">
+        <v>72</v>
+      </c>
+      <c r="D74" t="n">
+        <v>72</v>
+      </c>
+      <c r="E74" t="inlineStr">
         <is>
           <t>Crushed Red</t>
         </is>
       </c>
-      <c r="C74" t="n">
-        <v>1</v>
-      </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B75" t="n">
+        <v>73</v>
+      </c>
+      <c r="C75" t="n">
+        <v>73</v>
+      </c>
+      <c r="D75" t="n">
+        <v>73</v>
+      </c>
+      <c r="E75" t="inlineStr">
         <is>
           <t>Noodle's and Co</t>
         </is>
       </c>
-      <c r="C75" t="n">
-        <v>1</v>
-      </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B76" t="n">
+        <v>74</v>
+      </c>
+      <c r="C76" t="n">
+        <v>74</v>
+      </c>
+      <c r="D76" t="n">
+        <v>74</v>
+      </c>
+      <c r="E76" t="inlineStr">
         <is>
           <t>Copper Chimney</t>
         </is>
       </c>
-      <c r="C76" t="n">
-        <v>1</v>
-      </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B77" t="n">
+        <v>75</v>
+      </c>
+      <c r="C77" t="n">
+        <v>75</v>
+      </c>
+      <c r="D77" t="n">
+        <v>75</v>
+      </c>
+      <c r="E77" t="inlineStr">
         <is>
           <t xml:space="preserve">Indian Aroma </t>
         </is>
       </c>
-      <c r="C77" t="n">
-        <v>1</v>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B78" t="n">
+        <v>76</v>
+      </c>
+      <c r="C78" t="n">
+        <v>76</v>
+      </c>
+      <c r="D78" t="n">
+        <v>76</v>
+      </c>
+      <c r="E78" t="inlineStr">
         <is>
           <t>The Curry Club</t>
         </is>
       </c>
-      <c r="C78" t="n">
-        <v>2</v>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="n">
+        <v>2</v>
+      </c>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B79" t="n">
+        <v>77</v>
+      </c>
+      <c r="C79" t="n">
+        <v>77</v>
+      </c>
+      <c r="D79" t="n">
+        <v>77</v>
+      </c>
+      <c r="E79" t="inlineStr">
         <is>
           <t>Strange Donuts</t>
         </is>
       </c>
-      <c r="C79" t="n">
+      <c r="F79" t="n">
         <v>6</v>
       </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="B80" t="n">
+        <v>78</v>
+      </c>
+      <c r="C80" t="n">
+        <v>78</v>
+      </c>
+      <c r="D80" t="n">
+        <v>78</v>
+      </c>
+      <c r="E80" t="inlineStr">
         <is>
           <t>Duck Donuts</t>
         </is>
       </c>
-      <c r="C80" t="n">
+      <c r="F80" t="n">
         <v>6</v>
       </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B81" t="n">
+        <v>79</v>
+      </c>
+      <c r="C81" t="n">
+        <v>79</v>
+      </c>
+      <c r="D81" t="n">
+        <v>79</v>
+      </c>
+      <c r="E81" t="inlineStr">
         <is>
           <t>Donut King</t>
         </is>
       </c>
-      <c r="C81" t="n">
+      <c r="F81" t="n">
         <v>6</v>
       </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B82" t="n">
+        <v>80</v>
+      </c>
+      <c r="C82" t="n">
+        <v>80</v>
+      </c>
+      <c r="D82" t="n">
+        <v>80</v>
+      </c>
+      <c r="E82" t="inlineStr">
         <is>
           <t>Shake Shack</t>
         </is>
       </c>
-      <c r="C82" t="n">
-        <v>1</v>
-      </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B83" t="n">
+        <v>81</v>
+      </c>
+      <c r="C83" t="n">
+        <v>81</v>
+      </c>
+      <c r="D83" t="n">
+        <v>81</v>
+      </c>
+      <c r="E83" t="inlineStr">
         <is>
           <t>Buffalo Wild Wings</t>
         </is>
       </c>
-      <c r="C83" t="n">
-        <v>1</v>
-      </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B84" t="n">
+        <v>82</v>
+      </c>
+      <c r="C84" t="n">
+        <v>82</v>
+      </c>
+      <c r="D84" t="n">
+        <v>82</v>
+      </c>
+      <c r="E84" t="inlineStr">
         <is>
           <t>The Gelateria</t>
         </is>
       </c>
-      <c r="C84" t="n">
+      <c r="F84" t="n">
         <v>4</v>
       </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B85" t="n">
+        <v>83</v>
+      </c>
+      <c r="C85" t="n">
+        <v>83</v>
+      </c>
+      <c r="D85" t="n">
+        <v>83</v>
+      </c>
+      <c r="E85" t="inlineStr">
         <is>
           <t>Lulu's Local Eatery</t>
         </is>
       </c>
-      <c r="C85" t="n">
-        <v>2</v>
-      </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="n">
+        <v>2</v>
+      </c>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B86" t="n">
+        <v>84</v>
+      </c>
+      <c r="C86" t="n">
+        <v>84</v>
+      </c>
+      <c r="D86" t="n">
+        <v>84</v>
+      </c>
+      <c r="E86" t="inlineStr">
         <is>
           <t>Treehouse</t>
         </is>
       </c>
-      <c r="C86" t="n">
-        <v>2</v>
-      </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="n">
+        <v>2</v>
+      </c>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B87" t="n">
+        <v>85</v>
+      </c>
+      <c r="C87" t="n">
+        <v>85</v>
+      </c>
+      <c r="D87" t="n">
+        <v>85</v>
+      </c>
+      <c r="E87" t="inlineStr">
         <is>
           <t>Basil Spice</t>
         </is>
       </c>
-      <c r="C87" t="n">
-        <v>2</v>
-      </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="n">
+        <v>2</v>
+      </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B88" t="n">
+        <v>86</v>
+      </c>
+      <c r="C88" t="n">
+        <v>86</v>
+      </c>
+      <c r="D88" t="n">
+        <v>86</v>
+      </c>
+      <c r="E88" t="inlineStr">
         <is>
           <t>Sheesh</t>
         </is>
       </c>
-      <c r="C88" t="n">
-        <v>2</v>
-      </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="n">
+        <v>2</v>
+      </c>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B89" t="n">
+        <v>87</v>
+      </c>
+      <c r="C89" t="n">
+        <v>87</v>
+      </c>
+      <c r="D89" t="n">
+        <v>87</v>
+      </c>
+      <c r="E89" t="inlineStr">
         <is>
           <t>Kevlar Coffee</t>
         </is>
       </c>
-      <c r="C89" t="n">
+      <c r="F89" t="n">
         <v>4</v>
       </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B90" t="n">
+        <v>88</v>
+      </c>
+      <c r="C90" t="n">
+        <v>88</v>
+      </c>
+      <c r="D90" t="n">
+        <v>88</v>
+      </c>
+      <c r="E90" t="inlineStr">
         <is>
           <t>Cornerstone Coffee</t>
         </is>
       </c>
-      <c r="C90" t="n">
+      <c r="F90" t="n">
         <v>4</v>
       </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="B91" t="n">
+        <v>89</v>
+      </c>
+      <c r="C91" t="n">
+        <v>89</v>
+      </c>
+      <c r="D91" t="n">
+        <v>89</v>
+      </c>
+      <c r="E91" t="inlineStr">
         <is>
           <t>Comet Coffee</t>
         </is>
       </c>
-      <c r="C91" t="n">
+      <c r="F91" t="n">
         <v>4</v>
       </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B92" t="inlineStr">
+      <c r="B92" t="n">
+        <v>90</v>
+      </c>
+      <c r="C92" t="n">
+        <v>90</v>
+      </c>
+      <c r="D92" t="n">
+        <v>90</v>
+      </c>
+      <c r="E92" t="inlineStr">
         <is>
           <t>Peace Love Coffee (V)</t>
         </is>
       </c>
-      <c r="C92" t="n">
-        <v>2</v>
-      </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="B93" t="n">
+        <v>91</v>
+      </c>
+      <c r="C93" t="n">
+        <v>91</v>
+      </c>
+      <c r="D93" t="n">
+        <v>91</v>
+      </c>
+      <c r="E93" t="inlineStr">
         <is>
           <t>Seedz Cafe (V)</t>
         </is>
       </c>
-      <c r="C93" t="n">
-        <v>2</v>
-      </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
+      <c r="F93" t="n">
+        <v>2</v>
+      </c>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="B94" t="n">
+        <v>92</v>
+      </c>
+      <c r="C94" t="n">
+        <v>92</v>
+      </c>
+      <c r="D94" t="n">
+        <v>92</v>
+      </c>
+      <c r="E94" t="inlineStr">
         <is>
           <t>Bubblecup Tea Zone</t>
         </is>
       </c>
-      <c r="C94" t="n">
+      <c r="F94" t="n">
         <v>4</v>
       </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="B95" t="n">
+        <v>93</v>
+      </c>
+      <c r="C95" t="n">
+        <v>93</v>
+      </c>
+      <c r="D95" t="n">
+        <v>93</v>
+      </c>
+      <c r="E95" t="inlineStr">
         <is>
           <t>Mudslinger's Coffee</t>
         </is>
       </c>
-      <c r="C95" t="n">
+      <c r="F95" t="n">
         <v>4</v>
       </c>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B96" t="inlineStr">
+      <c r="B96" t="n">
+        <v>94</v>
+      </c>
+      <c r="C96" t="n">
+        <v>94</v>
+      </c>
+      <c r="D96" t="n">
+        <v>94</v>
+      </c>
+      <c r="E96" t="inlineStr">
         <is>
           <t>The Original Pancake House</t>
         </is>
       </c>
-      <c r="C96" t="n">
+      <c r="F96" t="n">
         <v>6</v>
       </c>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B97" t="inlineStr">
+      <c r="B97" t="n">
+        <v>95</v>
+      </c>
+      <c r="C97" t="n">
+        <v>95</v>
+      </c>
+      <c r="D97" t="n">
+        <v>95</v>
+      </c>
+      <c r="E97" t="inlineStr">
         <is>
           <t>First Watch</t>
         </is>
       </c>
-      <c r="C97" t="n">
+      <c r="F97" t="n">
         <v>6</v>
       </c>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98" t="inlineStr">
+      <c r="B98" t="n">
+        <v>96</v>
+      </c>
+      <c r="C98" t="n">
+        <v>96</v>
+      </c>
+      <c r="D98" t="n">
+        <v>96</v>
+      </c>
+      <c r="E98" t="inlineStr">
         <is>
           <t>The Shack</t>
         </is>
       </c>
-      <c r="C98" t="n">
+      <c r="F98" t="n">
         <v>6</v>
       </c>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B99" t="n">
+        <v>97</v>
+      </c>
+      <c r="C99" t="n">
+        <v>97</v>
+      </c>
+      <c r="D99" t="n">
+        <v>97</v>
+      </c>
+      <c r="E99" t="inlineStr">
         <is>
           <t>Jafra</t>
         </is>
       </c>
-      <c r="C99" t="n">
-        <v>1</v>
-      </c>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="n">
+        <v>1</v>
+      </c>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B100" t="inlineStr">
+      <c r="B100" t="n">
+        <v>98</v>
+      </c>
+      <c r="C100" t="n">
+        <v>98</v>
+      </c>
+      <c r="D100" t="n">
+        <v>98</v>
+      </c>
+      <c r="E100" t="inlineStr">
         <is>
           <t>Tango Argentina</t>
         </is>
       </c>
-      <c r="C100" t="n">
-        <v>2</v>
-      </c>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="n">
+        <v>2</v>
+      </c>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B101" t="inlineStr">
+      <c r="B101" t="n">
+        <v>99</v>
+      </c>
+      <c r="C101" t="n">
+        <v>99</v>
+      </c>
+      <c r="D101" t="n">
+        <v>99</v>
+      </c>
+      <c r="E101" t="inlineStr">
         <is>
           <t>Fuzzy's Tacos</t>
         </is>
       </c>
-      <c r="C101" t="n">
-        <v>2</v>
-      </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B102" t="inlineStr">
+      <c r="B102" t="n">
+        <v>100</v>
+      </c>
+      <c r="C102" t="n">
+        <v>100</v>
+      </c>
+      <c r="D102" t="n">
+        <v>100</v>
+      </c>
+      <c r="E102" t="inlineStr">
         <is>
           <t>Lee's Chicken</t>
         </is>
       </c>
-      <c r="C102" t="n">
-        <v>2</v>
-      </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="n">
+        <v>2</v>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B103" t="inlineStr">
+      <c r="B103" t="n">
+        <v>101</v>
+      </c>
+      <c r="C103" t="n">
+        <v>101</v>
+      </c>
+      <c r="D103" t="n">
+        <v>101</v>
+      </c>
+      <c r="E103" t="inlineStr">
         <is>
           <t>P.F. Chang's</t>
         </is>
       </c>
-      <c r="C103" t="n">
-        <v>2</v>
-      </c>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="n">
+        <v>2</v>
+      </c>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B104" t="inlineStr">
+      <c r="B104" t="n">
+        <v>102</v>
+      </c>
+      <c r="C104" t="n">
+        <v>102</v>
+      </c>
+      <c r="D104" t="n">
+        <v>102</v>
+      </c>
+      <c r="E104" t="inlineStr">
         <is>
           <t>Loaded Nacho's</t>
         </is>
       </c>
-      <c r="C104" t="n">
-        <v>2</v>
-      </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="n">
+        <v>2</v>
+      </c>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B105" t="inlineStr">
+      <c r="B105" t="n">
+        <v>103</v>
+      </c>
+      <c r="C105" t="n">
+        <v>103</v>
+      </c>
+      <c r="D105" t="n">
+        <v>103</v>
+      </c>
+      <c r="E105" t="inlineStr">
         <is>
           <t xml:space="preserve">Narwhal's </t>
         </is>
       </c>
-      <c r="C105" t="n">
+      <c r="F105" t="n">
         <v>5</v>
       </c>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B106" t="inlineStr">
+      <c r="B106" t="n">
+        <v>104</v>
+      </c>
+      <c r="C106" t="n">
+        <v>104</v>
+      </c>
+      <c r="D106" t="n">
+        <v>104</v>
+      </c>
+      <c r="E106" t="inlineStr">
         <is>
           <t xml:space="preserve">Massa's </t>
         </is>
       </c>
-      <c r="C106" t="n">
+      <c r="F106" t="n">
         <v>5</v>
       </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="B107" t="inlineStr">
+      <c r="B107" t="n">
+        <v>105</v>
+      </c>
+      <c r="C107" t="n">
+        <v>105</v>
+      </c>
+      <c r="D107" t="n">
+        <v>105</v>
+      </c>
+      <c r="E107" t="inlineStr">
         <is>
           <t>Q64</t>
         </is>
       </c>
-      <c r="C107" t="n">
+      <c r="F107" t="n">
         <v>5</v>
       </c>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="B108" t="inlineStr">
+      <c r="B108" t="n">
+        <v>106</v>
+      </c>
+      <c r="C108" t="n">
+        <v>106</v>
+      </c>
+      <c r="D108" t="n">
+        <v>106</v>
+      </c>
+      <c r="E108" t="inlineStr">
         <is>
           <t>Seoul Taco</t>
         </is>
       </c>
-      <c r="C108" t="n">
-        <v>2</v>
-      </c>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="n">
+        <v>2</v>
+      </c>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="B109" t="inlineStr">
+      <c r="B109" t="n">
+        <v>107</v>
+      </c>
+      <c r="C109" t="n">
+        <v>107</v>
+      </c>
+      <c r="D109" t="n">
+        <v>107</v>
+      </c>
+      <c r="E109" t="inlineStr">
         <is>
           <t>Rehab</t>
         </is>
       </c>
-      <c r="C109" t="n">
+      <c r="F109" t="n">
         <v>5</v>
       </c>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="inlineStr"/>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="B110" t="inlineStr">
+      <c r="B110" t="n">
+        <v>108</v>
+      </c>
+      <c r="C110" t="n">
+        <v>108</v>
+      </c>
+      <c r="D110" t="n">
+        <v>108</v>
+      </c>
+      <c r="E110" t="inlineStr">
         <is>
           <t>Pizza Head</t>
         </is>
       </c>
-      <c r="C110" t="n">
-        <v>2</v>
-      </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="n">
+        <v>2</v>
+      </c>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="B111" t="inlineStr">
+      <c r="B111" t="n">
+        <v>109</v>
+      </c>
+      <c r="C111" t="n">
+        <v>109</v>
+      </c>
+      <c r="D111" t="n">
+        <v>109</v>
+      </c>
+      <c r="E111" t="inlineStr">
         <is>
           <t>Blackbear Diner</t>
         </is>
       </c>
-      <c r="C111" t="n">
-        <v>2</v>
-      </c>
-      <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="n">
+        <v>2</v>
+      </c>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="B112" t="inlineStr">
+      <c r="B112" t="n">
+        <v>110</v>
+      </c>
+      <c r="C112" t="n">
+        <v>110</v>
+      </c>
+      <c r="D112" t="n">
+        <v>110</v>
+      </c>
+      <c r="E112" t="inlineStr">
         <is>
           <t>Goodnews Brewing</t>
         </is>
       </c>
-      <c r="C112" t="n">
+      <c r="F112" t="n">
         <v>5</v>
       </c>
-      <c r="D112" t="inlineStr"/>
-      <c r="E112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="B113" t="inlineStr">
+      <c r="B113" t="n">
+        <v>111</v>
+      </c>
+      <c r="C113" t="n">
+        <v>111</v>
+      </c>
+      <c r="D113" t="n">
+        <v>111</v>
+      </c>
+      <c r="E113" t="inlineStr">
         <is>
           <t>Small Batch Winery</t>
         </is>
       </c>
-      <c r="C113" t="n">
+      <c r="F113" t="n">
         <v>5</v>
       </c>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="B114" t="inlineStr">
+      <c r="B114" t="n">
+        <v>112</v>
+      </c>
+      <c r="C114" t="n">
+        <v>112</v>
+      </c>
+      <c r="D114" t="n">
+        <v>112</v>
+      </c>
+      <c r="E114" t="inlineStr">
         <is>
           <t>Quarry Wine Garden</t>
         </is>
       </c>
-      <c r="C114" t="n">
+      <c r="F114" t="n">
         <v>5</v>
       </c>
-      <c r="D114" t="inlineStr"/>
-      <c r="E114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="B115" t="inlineStr">
+      <c r="B115" t="n">
+        <v>113</v>
+      </c>
+      <c r="C115" t="n">
+        <v>113</v>
+      </c>
+      <c r="D115" t="n">
+        <v>113</v>
+      </c>
+      <c r="E115" t="inlineStr">
         <is>
           <t>Kitaro</t>
         </is>
       </c>
-      <c r="C115" t="n">
-        <v>2</v>
-      </c>
-      <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="n">
+        <v>2</v>
+      </c>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="B116" t="inlineStr">
+      <c r="B116" t="n">
+        <v>114</v>
+      </c>
+      <c r="C116" t="n">
+        <v>114</v>
+      </c>
+      <c r="D116" t="n">
+        <v>114</v>
+      </c>
+      <c r="E116" t="inlineStr">
         <is>
           <t>Tully's Taproom</t>
         </is>
       </c>
-      <c r="C116" t="n">
+      <c r="F116" t="n">
         <v>5</v>
       </c>
-      <c r="D116" t="inlineStr"/>
-      <c r="E116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B117" t="inlineStr">
+      <c r="B117" t="n">
+        <v>115</v>
+      </c>
+      <c r="C117" t="n">
+        <v>115</v>
+      </c>
+      <c r="D117" t="n">
+        <v>115</v>
+      </c>
+      <c r="E117" t="inlineStr">
         <is>
           <t>A'mis Pizza</t>
         </is>
       </c>
-      <c r="C117" t="n">
-        <v>1</v>
-      </c>
-      <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="n">
+        <v>1</v>
+      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B118" t="inlineStr">
+      <c r="B118" t="n">
+        <v>116</v>
+      </c>
+      <c r="C118" t="n">
+        <v>116</v>
+      </c>
+      <c r="D118" t="n">
+        <v>116</v>
+      </c>
+      <c r="E118" t="inlineStr">
         <is>
           <t>Bandana's</t>
         </is>
       </c>
-      <c r="C118" t="n">
-        <v>1</v>
-      </c>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="n">
+        <v>1</v>
+      </c>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="B119" t="inlineStr">
+      <c r="B119" t="n">
+        <v>117</v>
+      </c>
+      <c r="C119" t="n">
+        <v>117</v>
+      </c>
+      <c r="D119" t="n">
+        <v>117</v>
+      </c>
+      <c r="E119" t="inlineStr">
         <is>
           <t>Scooter's Coffee</t>
         </is>
       </c>
-      <c r="C119" t="n">
+      <c r="F119" t="n">
         <v>4</v>
       </c>
-      <c r="D119" t="inlineStr"/>
-      <c r="E119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="B120" t="inlineStr">
+      <c r="B120" t="n">
+        <v>118</v>
+      </c>
+      <c r="C120" t="n">
+        <v>118</v>
+      </c>
+      <c r="D120" t="n">
+        <v>118</v>
+      </c>
+      <c r="E120" t="inlineStr">
         <is>
           <t>Dogwood Social House</t>
         </is>
       </c>
-      <c r="C120" t="n">
+      <c r="F120" t="n">
         <v>5</v>
       </c>
-      <c r="D120" t="inlineStr"/>
-      <c r="E120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="B121" t="inlineStr">
+      <c r="B121" t="n">
+        <v>119</v>
+      </c>
+      <c r="C121" t="n">
+        <v>119</v>
+      </c>
+      <c r="D121" t="n">
+        <v>119</v>
+      </c>
+      <c r="E121" t="inlineStr">
         <is>
           <t>STL Kolache</t>
         </is>
       </c>
-      <c r="C121" t="n">
+      <c r="F121" t="n">
         <v>6</v>
       </c>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B122" t="inlineStr">
+      <c r="B122" t="n">
+        <v>120</v>
+      </c>
+      <c r="C122" t="n">
+        <v>120</v>
+      </c>
+      <c r="D122" t="n">
+        <v>120</v>
+      </c>
+      <c r="E122" t="inlineStr">
         <is>
           <t>Oberweis</t>
         </is>
       </c>
-      <c r="C122" t="n">
+      <c r="F122" t="n">
         <v>3</v>
       </c>
-      <c r="D122" t="inlineStr"/>
-      <c r="E122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="B123" t="inlineStr">
+      <c r="B123" t="n">
+        <v>121</v>
+      </c>
+      <c r="C123" t="n">
+        <v>121</v>
+      </c>
+      <c r="D123" t="n">
+        <v>121</v>
+      </c>
+      <c r="E123" t="inlineStr">
         <is>
           <t>Woodgrain Pizzeria</t>
         </is>
       </c>
-      <c r="C123" t="n">
-        <v>1</v>
-      </c>
-      <c r="D123" t="inlineStr"/>
-      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="n">
+        <v>1</v>
+      </c>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="B124" t="inlineStr">
+      <c r="B124" t="n">
+        <v>122</v>
+      </c>
+      <c r="C124" t="n">
+        <v>122</v>
+      </c>
+      <c r="D124" t="n">
+        <v>122</v>
+      </c>
+      <c r="E124" t="inlineStr">
         <is>
           <t>That Burger Joint</t>
         </is>
       </c>
-      <c r="C124" t="n">
-        <v>1</v>
-      </c>
-      <c r="D124" t="inlineStr"/>
-      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="n">
+        <v>1</v>
+      </c>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="B125" t="inlineStr">
+      <c r="B125" t="n">
+        <v>123</v>
+      </c>
+      <c r="C125" t="n">
+        <v>123</v>
+      </c>
+      <c r="D125" t="n">
+        <v>123</v>
+      </c>
+      <c r="E125" t="inlineStr">
         <is>
           <t>Mellow Mushroom</t>
         </is>
       </c>
-      <c r="C125" t="n">
-        <v>1</v>
-      </c>
-      <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="n">
+        <v>1</v>
+      </c>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="B126" t="inlineStr">
+      <c r="B126" t="n">
+        <v>124</v>
+      </c>
+      <c r="C126" t="n">
+        <v>124</v>
+      </c>
+      <c r="D126" t="n">
+        <v>124</v>
+      </c>
+      <c r="E126" t="inlineStr">
         <is>
           <t>Smoothie King</t>
         </is>
       </c>
-      <c r="C126" t="n">
-        <v>1</v>
-      </c>
-      <c r="D126" t="inlineStr"/>
-      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="n">
+        <v>1</v>
+      </c>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="B127" t="inlineStr">
+      <c r="B127" t="n">
+        <v>125</v>
+      </c>
+      <c r="C127" t="n">
+        <v>125</v>
+      </c>
+      <c r="D127" t="n">
+        <v>125</v>
+      </c>
+      <c r="E127" t="inlineStr">
         <is>
           <t>Smoothie King</t>
         </is>
       </c>
-      <c r="C127" t="n">
+      <c r="F127" t="n">
         <v>3</v>
       </c>
-      <c r="D127" t="inlineStr"/>
-      <c r="E127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="B128" t="inlineStr">
+      <c r="B128" t="n">
+        <v>126</v>
+      </c>
+      <c r="C128" t="n">
+        <v>126</v>
+      </c>
+      <c r="D128" t="n">
+        <v>126</v>
+      </c>
+      <c r="E128" t="inlineStr">
         <is>
           <t xml:space="preserve">Pantera's </t>
         </is>
       </c>
-      <c r="C128" t="n">
-        <v>1</v>
-      </c>
-      <c r="D128" t="inlineStr"/>
-      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="n">
+        <v>1</v>
+      </c>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="B129" t="inlineStr">
+      <c r="B129" t="n">
+        <v>127</v>
+      </c>
+      <c r="C129" t="n">
+        <v>127</v>
+      </c>
+      <c r="D129" t="n">
+        <v>127</v>
+      </c>
+      <c r="E129" t="inlineStr">
         <is>
           <t xml:space="preserve">Monical's </t>
         </is>
       </c>
-      <c r="C129" t="n">
-        <v>1</v>
-      </c>
-      <c r="D129" t="inlineStr"/>
-      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="n">
+        <v>1</v>
+      </c>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="B130" t="inlineStr">
+      <c r="B130" t="n">
+        <v>128</v>
+      </c>
+      <c r="C130" t="n">
+        <v>128</v>
+      </c>
+      <c r="D130" t="n">
+        <v>128</v>
+      </c>
+      <c r="E130" t="inlineStr">
         <is>
           <t xml:space="preserve">Ethyl's </t>
         </is>
       </c>
-      <c r="C130" t="n">
-        <v>2</v>
-      </c>
-      <c r="D130" t="inlineStr"/>
-      <c r="E130" t="inlineStr"/>
+      <c r="F130" t="n">
+        <v>2</v>
+      </c>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="B131" t="inlineStr">
+      <c r="B131" t="n">
+        <v>129</v>
+      </c>
+      <c r="C131" t="n">
+        <v>129</v>
+      </c>
+      <c r="D131" t="n">
+        <v>129</v>
+      </c>
+      <c r="E131" t="inlineStr">
         <is>
           <t>Baskin-Robbins</t>
         </is>
       </c>
-      <c r="C131" t="n">
+      <c r="F131" t="n">
         <v>3</v>
       </c>
-      <c r="D131" t="inlineStr"/>
-      <c r="E131" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="B132" t="inlineStr">
+      <c r="B132" t="n">
+        <v>130</v>
+      </c>
+      <c r="C132" t="n">
+        <v>130</v>
+      </c>
+      <c r="D132" t="n">
+        <v>130</v>
+      </c>
+      <c r="E132" t="inlineStr">
         <is>
           <t>Cheesecake Factory</t>
         </is>
       </c>
-      <c r="C132" t="n">
+      <c r="F132" t="n">
         <v>3</v>
       </c>
-      <c r="D132" t="inlineStr"/>
-      <c r="E132" t="inlineStr"/>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="B133" t="inlineStr">
+      <c r="B133" t="n">
+        <v>131</v>
+      </c>
+      <c r="C133" t="n">
+        <v>131</v>
+      </c>
+      <c r="D133" t="n">
+        <v>131</v>
+      </c>
+      <c r="E133" t="inlineStr">
         <is>
           <t>Rally's</t>
         </is>
       </c>
-      <c r="C133" t="n">
-        <v>1</v>
-      </c>
-      <c r="D133" t="inlineStr"/>
-      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="n">
+        <v>1</v>
+      </c>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="B134" t="inlineStr">
+      <c r="B134" t="n">
+        <v>132</v>
+      </c>
+      <c r="C134" t="n">
+        <v>132</v>
+      </c>
+      <c r="D134" t="n">
+        <v>132</v>
+      </c>
+      <c r="E134" t="inlineStr">
         <is>
           <t>Rendezvous Cafe and Wine Bar</t>
         </is>
       </c>
-      <c r="C134" t="n">
+      <c r="F134" t="n">
         <v>5</v>
       </c>
-      <c r="D134" t="inlineStr"/>
-      <c r="E134" t="inlineStr"/>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="B135" t="inlineStr">
+      <c r="B135" t="n">
+        <v>133</v>
+      </c>
+      <c r="C135" t="n">
+        <v>133</v>
+      </c>
+      <c r="D135" t="n">
+        <v>133</v>
+      </c>
+      <c r="E135" t="inlineStr">
         <is>
           <t>Silky's</t>
         </is>
       </c>
-      <c r="C135" t="n">
+      <c r="F135" t="n">
         <v>3</v>
       </c>
-      <c r="D135" t="inlineStr"/>
-      <c r="E135" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="B136" t="inlineStr">
+      <c r="B136" t="n">
+        <v>134</v>
+      </c>
+      <c r="C136" t="n">
+        <v>134</v>
+      </c>
+      <c r="D136" t="n">
+        <v>134</v>
+      </c>
+      <c r="E136" t="inlineStr">
         <is>
           <t>Lulu's Bar and Grill</t>
         </is>
       </c>
-      <c r="C136" t="n">
-        <v>2</v>
-      </c>
-      <c r="D136" t="inlineStr"/>
-      <c r="E136" t="inlineStr"/>
+      <c r="F136" t="n">
+        <v>2</v>
+      </c>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="B137" t="inlineStr">
+      <c r="B137" t="n">
+        <v>135</v>
+      </c>
+      <c r="C137" t="n">
+        <v>135</v>
+      </c>
+      <c r="D137" t="n">
+        <v>135</v>
+      </c>
+      <c r="E137" t="inlineStr">
         <is>
           <t>Bahama Buck's</t>
         </is>
       </c>
-      <c r="C137" t="n">
+      <c r="F137" t="n">
         <v>3</v>
       </c>
-      <c r="D137" t="inlineStr"/>
-      <c r="E137" t="inlineStr"/>
+      <c r="G137" t="inlineStr"/>
+      <c r="H137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="B138" t="inlineStr">
+      <c r="B138" t="n">
+        <v>136</v>
+      </c>
+      <c r="C138" t="n">
+        <v>136</v>
+      </c>
+      <c r="D138" t="n">
+        <v>136</v>
+      </c>
+      <c r="E138" t="inlineStr">
         <is>
           <t>Crumbl Cookies</t>
         </is>
       </c>
-      <c r="C138" t="n">
+      <c r="F138" t="n">
         <v>3</v>
       </c>
-      <c r="D138" t="inlineStr"/>
-      <c r="E138" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="B139" t="inlineStr">
+      <c r="B139" t="n">
+        <v>137</v>
+      </c>
+      <c r="C139" t="n">
+        <v>137</v>
+      </c>
+      <c r="D139" t="n">
+        <v>137</v>
+      </c>
+      <c r="E139" t="inlineStr">
         <is>
           <t>Smashburger</t>
         </is>
       </c>
-      <c r="C139" t="n">
-        <v>1</v>
-      </c>
-      <c r="D139" t="inlineStr"/>
-      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="n">
+        <v>1</v>
+      </c>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="B140" t="inlineStr">
+      <c r="B140" t="n">
+        <v>138</v>
+      </c>
+      <c r="C140" t="n">
+        <v>138</v>
+      </c>
+      <c r="D140" t="n">
+        <v>138</v>
+      </c>
+      <c r="E140" t="inlineStr">
         <is>
           <t>Cork and Rind</t>
         </is>
       </c>
-      <c r="C140" t="n">
+      <c r="F140" t="n">
         <v>5</v>
       </c>
-      <c r="D140" t="inlineStr"/>
-      <c r="E140" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="B141" t="inlineStr">
+      <c r="B141" t="n">
+        <v>139</v>
+      </c>
+      <c r="C141" t="n">
+        <v>139</v>
+      </c>
+      <c r="D141" t="n">
+        <v>139</v>
+      </c>
+      <c r="E141" t="inlineStr">
         <is>
           <t>Four Hands Brewing</t>
         </is>
       </c>
-      <c r="C141" t="n">
+      <c r="F141" t="n">
         <v>5</v>
       </c>
-      <c r="D141" t="inlineStr"/>
-      <c r="E141" t="inlineStr"/>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="B142" t="inlineStr">
+      <c r="B142" t="n">
+        <v>140</v>
+      </c>
+      <c r="C142" t="n">
+        <v>140</v>
+      </c>
+      <c r="D142" t="n">
+        <v>140</v>
+      </c>
+      <c r="E142" t="inlineStr">
         <is>
           <t>Bike Stop Cafe</t>
         </is>
       </c>
-      <c r="C142" t="n">
+      <c r="F142" t="n">
         <v>4</v>
       </c>
-      <c r="D142" t="inlineStr"/>
-      <c r="E142" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="B143" t="inlineStr">
+      <c r="B143" t="n">
+        <v>141</v>
+      </c>
+      <c r="C143" t="n">
+        <v>141</v>
+      </c>
+      <c r="D143" t="n">
+        <v>141</v>
+      </c>
+      <c r="E143" t="inlineStr">
         <is>
           <t>Kilwin's</t>
         </is>
       </c>
-      <c r="C143" t="n">
+      <c r="F143" t="n">
         <v>3</v>
       </c>
-      <c r="D143" t="inlineStr"/>
-      <c r="E143" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="B144" t="inlineStr">
+      <c r="B144" t="n">
+        <v>142</v>
+      </c>
+      <c r="C144" t="n">
+        <v>142</v>
+      </c>
+      <c r="D144" t="n">
+        <v>142</v>
+      </c>
+      <c r="E144" t="inlineStr">
         <is>
           <t>Bella Vino Wine Bar and Tapas</t>
         </is>
       </c>
-      <c r="C144" t="n">
+      <c r="F144" t="n">
         <v>5</v>
       </c>
-      <c r="D144" t="inlineStr"/>
-      <c r="E144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="B145" t="inlineStr">
+      <c r="B145" t="n">
+        <v>143</v>
+      </c>
+      <c r="C145" t="n">
+        <v>143</v>
+      </c>
+      <c r="D145" t="n">
+        <v>143</v>
+      </c>
+      <c r="E145" t="inlineStr">
         <is>
           <t xml:space="preserve">Llywelyn's </t>
         </is>
       </c>
-      <c r="C145" t="n">
+      <c r="F145" t="n">
         <v>5</v>
       </c>
-      <c r="D145" t="inlineStr"/>
-      <c r="E145" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="B146" t="inlineStr">
+      <c r="B146" t="n">
+        <v>144</v>
+      </c>
+      <c r="C146" t="n">
+        <v>144</v>
+      </c>
+      <c r="D146" t="n">
+        <v>144</v>
+      </c>
+      <c r="E146" t="inlineStr">
         <is>
           <t>Little O's Soda Shop</t>
         </is>
       </c>
-      <c r="C146" t="n">
+      <c r="F146" t="n">
         <v>3</v>
       </c>
-      <c r="D146" t="inlineStr"/>
-      <c r="E146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="B147" t="inlineStr">
+      <c r="B147" t="n">
+        <v>145</v>
+      </c>
+      <c r="C147" t="n">
+        <v>145</v>
+      </c>
+      <c r="D147" t="n">
+        <v>145</v>
+      </c>
+      <c r="E147" t="inlineStr">
         <is>
           <t>Rootbound (V)</t>
         </is>
       </c>
-      <c r="C147" t="n">
-        <v>2</v>
-      </c>
-      <c r="D147" t="inlineStr"/>
-      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="n">
+        <v>2</v>
+      </c>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="B148" t="inlineStr">
+      <c r="B148" t="n">
+        <v>146</v>
+      </c>
+      <c r="C148" t="n">
+        <v>146</v>
+      </c>
+      <c r="D148" t="n">
+        <v>146</v>
+      </c>
+      <c r="E148" t="inlineStr">
         <is>
           <t>The Baked Bear</t>
         </is>
       </c>
-      <c r="C148" t="n">
+      <c r="F148" t="n">
         <v>3</v>
       </c>
-      <c r="D148" t="inlineStr"/>
-      <c r="E148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
         <v>147</v>
       </c>
-      <c r="B149" t="inlineStr">
+      <c r="B149" t="n">
+        <v>147</v>
+      </c>
+      <c r="C149" t="n">
+        <v>147</v>
+      </c>
+      <c r="D149" t="n">
+        <v>147</v>
+      </c>
+      <c r="E149" t="inlineStr">
         <is>
           <t>Prasino</t>
         </is>
       </c>
-      <c r="C149" t="n">
-        <v>2</v>
-      </c>
-      <c r="D149" t="inlineStr"/>
-      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="n">
+        <v>2</v>
+      </c>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="B150" t="inlineStr">
+      <c r="B150" t="n">
+        <v>148</v>
+      </c>
+      <c r="C150" t="n">
+        <v>148</v>
+      </c>
+      <c r="D150" t="n">
+        <v>148</v>
+      </c>
+      <c r="E150" t="inlineStr">
         <is>
           <t>Napoli 3</t>
         </is>
       </c>
-      <c r="C150" t="n">
-        <v>2</v>
-      </c>
-      <c r="D150" t="inlineStr"/>
-      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="n">
+        <v>2</v>
+      </c>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="B151" t="inlineStr">
+      <c r="B151" t="n">
+        <v>149</v>
+      </c>
+      <c r="C151" t="n">
+        <v>149</v>
+      </c>
+      <c r="D151" t="n">
+        <v>149</v>
+      </c>
+      <c r="E151" t="inlineStr">
         <is>
           <t>Hot Box Cookies</t>
         </is>
       </c>
-      <c r="C151" t="n">
+      <c r="F151" t="n">
         <v>3</v>
       </c>
-      <c r="D151" t="inlineStr"/>
-      <c r="E151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="B152" t="inlineStr">
+      <c r="B152" t="n">
+        <v>150</v>
+      </c>
+      <c r="C152" t="n">
+        <v>150</v>
+      </c>
+      <c r="D152" t="n">
+        <v>150</v>
+      </c>
+      <c r="E152" t="inlineStr">
         <is>
           <t xml:space="preserve">Jersey Mike's </t>
         </is>
       </c>
-      <c r="C152" t="n">
-        <v>1</v>
-      </c>
-      <c r="D152" t="inlineStr"/>
-      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="n">
+        <v>1</v>
+      </c>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="B153" t="inlineStr">
+      <c r="B153" t="n">
+        <v>151</v>
+      </c>
+      <c r="C153" t="n">
+        <v>151</v>
+      </c>
+      <c r="D153" t="n">
+        <v>151</v>
+      </c>
+      <c r="E153" t="inlineStr">
         <is>
           <t>CheeBurger CheeBurger</t>
         </is>
       </c>
-      <c r="C153" t="n">
-        <v>1</v>
-      </c>
-      <c r="D153" t="inlineStr"/>
-      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="n">
+        <v>1</v>
+      </c>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="B154" t="inlineStr">
+      <c r="B154" t="n">
+        <v>152</v>
+      </c>
+      <c r="C154" t="n">
+        <v>152</v>
+      </c>
+      <c r="D154" t="n">
+        <v>152</v>
+      </c>
+      <c r="E154" t="inlineStr">
         <is>
           <t>California Pizza Kitchen</t>
         </is>
       </c>
-      <c r="C154" t="n">
-        <v>1</v>
-      </c>
-      <c r="D154" t="inlineStr"/>
-      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="n">
+        <v>1</v>
+      </c>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="B155" t="inlineStr">
+      <c r="B155" t="n">
+        <v>153</v>
+      </c>
+      <c r="C155" t="n">
+        <v>153</v>
+      </c>
+      <c r="D155" t="n">
+        <v>153</v>
+      </c>
+      <c r="E155" t="inlineStr">
         <is>
           <t>Coma Coffee</t>
         </is>
       </c>
-      <c r="C155" t="n">
+      <c r="F155" t="n">
         <v>4</v>
       </c>
-      <c r="D155" t="inlineStr"/>
-      <c r="E155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="B156" t="inlineStr">
+      <c r="B156" t="n">
+        <v>154</v>
+      </c>
+      <c r="C156" t="n">
+        <v>154</v>
+      </c>
+      <c r="D156" t="n">
+        <v>154</v>
+      </c>
+      <c r="E156" t="inlineStr">
         <is>
           <t>City Coffee and Creperie</t>
         </is>
       </c>
-      <c r="C156" t="n">
+      <c r="F156" t="n">
         <v>4</v>
       </c>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="B157" t="inlineStr">
+      <c r="B157" t="n">
+        <v>155</v>
+      </c>
+      <c r="C157" t="n">
+        <v>155</v>
+      </c>
+      <c r="D157" t="n">
+        <v>155</v>
+      </c>
+      <c r="E157" t="inlineStr">
         <is>
           <t>Jilly's Cupcakes</t>
         </is>
       </c>
-      <c r="C157" t="n">
+      <c r="F157" t="n">
         <v>3</v>
       </c>
-      <c r="D157" t="inlineStr"/>
-      <c r="E157" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="B158" t="inlineStr">
+      <c r="B158" t="n">
+        <v>156</v>
+      </c>
+      <c r="C158" t="n">
+        <v>156</v>
+      </c>
+      <c r="D158" t="n">
+        <v>156</v>
+      </c>
+      <c r="E158" t="inlineStr">
         <is>
           <t>Ballpark Village</t>
         </is>
       </c>
-      <c r="C158" t="n">
+      <c r="F158" t="n">
         <v>5</v>
       </c>
-      <c r="D158" t="inlineStr"/>
-      <c r="E158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="B159" t="inlineStr">
+      <c r="B159" t="n">
+        <v>157</v>
+      </c>
+      <c r="C159" t="n">
+        <v>157</v>
+      </c>
+      <c r="D159" t="n">
+        <v>157</v>
+      </c>
+      <c r="E159" t="inlineStr">
         <is>
           <t>Pie Guy</t>
         </is>
       </c>
-      <c r="C159" t="n">
-        <v>2</v>
-      </c>
-      <c r="D159" t="inlineStr"/>
-      <c r="E159" t="inlineStr"/>
+      <c r="F159" t="n">
+        <v>2</v>
+      </c>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="B160" t="inlineStr">
+      <c r="B160" t="n">
+        <v>158</v>
+      </c>
+      <c r="C160" t="n">
+        <v>158</v>
+      </c>
+      <c r="D160" t="n">
+        <v>158</v>
+      </c>
+      <c r="E160" t="inlineStr">
         <is>
           <t>Schlafly Tap Room</t>
         </is>
       </c>
-      <c r="C160" t="n">
+      <c r="F160" t="n">
         <v>5</v>
       </c>
-      <c r="D160" t="inlineStr"/>
-      <c r="E160" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="B161" t="inlineStr">
+      <c r="B161" t="n">
+        <v>159</v>
+      </c>
+      <c r="C161" t="n">
+        <v>159</v>
+      </c>
+      <c r="D161" t="n">
+        <v>159</v>
+      </c>
+      <c r="E161" t="inlineStr">
         <is>
           <t>Circle 7 Ranch</t>
         </is>
       </c>
-      <c r="C161" t="n">
+      <c r="F161" t="n">
         <v>5</v>
       </c>
-      <c r="D161" t="inlineStr"/>
-      <c r="E161" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="B162" t="inlineStr">
+      <c r="B162" t="n">
+        <v>160</v>
+      </c>
+      <c r="C162" t="n">
+        <v>160</v>
+      </c>
+      <c r="D162" t="n">
+        <v>160</v>
+      </c>
+      <c r="E162" t="inlineStr">
         <is>
           <t>City Foundry</t>
         </is>
       </c>
-      <c r="C162" t="n">
-        <v>2</v>
-      </c>
-      <c r="D162" t="inlineStr"/>
-      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="n">
+        <v>2</v>
+      </c>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="B163" t="inlineStr">
+      <c r="B163" t="n">
+        <v>161</v>
+      </c>
+      <c r="C163" t="n">
+        <v>161</v>
+      </c>
+      <c r="D163" t="n">
+        <v>161</v>
+      </c>
+      <c r="E163" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="C163" t="n">
+      <c r="F163" t="n">
         <v>3</v>
       </c>
-      <c r="D163" t="inlineStr"/>
-      <c r="E163" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>162</v>
+      </c>
+      <c r="C164" t="n">
+        <v>162</v>
+      </c>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>green china</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>1</v>
+      </c>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>163</v>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="F165" t="n">
+        <v>2</v>
+      </c>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>edit2</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>4</v>
+      </c>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added delete functionality for removing rows from excel sheet
</commit_message>
<xml_diff>
--- a/food_list.xlsx
+++ b/food_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H166"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4388,7 +4388,9 @@
       <c r="C164" t="n">
         <v>162</v>
       </c>
-      <c r="D164" t="inlineStr"/>
+      <c r="D164" t="n">
+        <v>162</v>
+      </c>
       <c r="E164" t="inlineStr">
         <is>
           <t>green china</t>
@@ -4402,41 +4404,27 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B165" t="n">
-        <v>163</v>
-      </c>
-      <c r="C165" t="inlineStr"/>
-      <c r="D165" t="inlineStr"/>
+        <v>164</v>
+      </c>
+      <c r="C165" t="n">
+        <v>164</v>
+      </c>
+      <c r="D165" t="n">
+        <v>164</v>
+      </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>edit</t>
+          <t>edit2</t>
         </is>
       </c>
       <c r="F165" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="inlineStr"/>
-    </row>
-    <row r="166">
-      <c r="A166" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="B166" t="inlineStr"/>
-      <c r="C166" t="inlineStr"/>
-      <c r="D166" t="inlineStr"/>
-      <c r="E166" t="inlineStr">
-        <is>
-          <t>edit2</t>
-        </is>
-      </c>
-      <c r="F166" t="n">
-        <v>4</v>
-      </c>
-      <c r="G166" t="inlineStr"/>
-      <c r="H166" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>